<commit_message>
Flight module unit test
</commit_message>
<xml_diff>
--- a/src/main/resources/dbAgencyTest.xlsx
+++ b/src/main/resources/dbAgencyTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Hoteles" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="DateFormatException" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="IsReservadoException" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="UpdateHotel" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="FlightDateFormatException" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="95">
   <si>
     <t xml:space="preserve">Código Hotel</t>
   </si>
@@ -157,54 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve">$7.320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TUPI-3369</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$12.530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$5.400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOCA-4213</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cartagena</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$8.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAME-0321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medellín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7.800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOBA-6567</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$57.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$39.860</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOME-4442</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$11.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEPI-9986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$41.640</t>
   </si>
   <si>
     <t xml:space="preserve">ESTOS DATOS SON PARA TENER UNA MUESTRA DE PERSONAS PARA PODER USAR EN LOS POST
@@ -335,6 +288,9 @@
   </si>
   <si>
     <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/0L/2021</t>
   </si>
   <si>
     <t>CH-0003</t>
@@ -366,8 +322,8 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="[$$-380A]#,##0.00;[RED]\([$$-380A]#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="168" formatCode="#,##0"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -490,7 +446,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -523,7 +479,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,31 +503,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -638,11 +590,11 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="2" customWidth="true" hidden="false" style="0" width="24.29" collapsed="true" outlineLevel="0"/>
     <col min="3" max="3" customWidth="true" hidden="false" style="0" width="18.86" collapsed="true" outlineLevel="0"/>
@@ -805,13 +757,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" customWidth="true" hidden="false" style="0" width="19.57" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="0" width="17.86" collapsed="true" outlineLevel="0"/>
@@ -912,7 +864,7 @@
         <v>44248</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -935,190 +887,17 @@
         <v>44244</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>44239</v>
-      </c>
-      <c r="G6" s="4" t="n">
-        <v>44250</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <v>44198</v>
-      </c>
-      <c r="G7" s="4" t="n">
-        <v>44212</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>44219</v>
-      </c>
-      <c r="G8" s="11" t="n">
-        <v>44232</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>44219</v>
-      </c>
-      <c r="G9" s="11" t="n">
-        <v>44227</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="4" t="n">
-        <v>44242</v>
-      </c>
-      <c r="G10" s="4" t="n">
-        <v>44255</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="4" t="n">
-        <v>44256</v>
-      </c>
-      <c r="G11" s="4" t="n">
-        <v>44269</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="4" t="n">
-        <v>44237</v>
-      </c>
-      <c r="G12" s="4" t="n">
-        <v>44251</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="4" t="n">
-        <v>44303</v>
-      </c>
-      <c r="G13" s="4" t="n">
-        <v>44318</v>
-      </c>
-    </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1141,247 +920,247 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="4" max="4" customWidth="true" hidden="false" style="0" width="25.71" collapsed="true" outlineLevel="0"/>
     <col min="5" max="5" customWidth="true" hidden="false" style="0" width="46.57" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="A1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="n">
+      <c r="A4" s="10" t="n">
         <v>12345678</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D4" s="11" t="n">
         <v>22214</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="n">
+      <c r="A5" s="10" t="n">
         <v>87654321</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>41376</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="n">
+      <c r="A6" s="10" t="n">
         <v>21553224</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>27977</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="n">
+      <c r="A7" s="10" t="n">
         <v>31501244</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>42090</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="n">
+      <c r="A8" s="12" t="n">
         <v>36061558</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="16" t="n">
+      <c r="B8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="14" t="n">
         <v>33931</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="n">
+      <c r="A9" s="10" t="n">
         <v>40555699</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>35992</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="n">
+      <c r="A10" s="10" t="n">
         <v>26554220</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>30952</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="n">
+      <c r="A11" s="10" t="n">
         <v>25333213</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="D11" s="4" t="n">
         <v>29862</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="n">
+      <c r="A12" s="10" t="n">
         <v>32556572</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>33431</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="n">
+      <c r="A13" s="10" t="n">
         <v>19558669</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>31083</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="n">
+      <c r="A14" s="10" t="n">
         <v>18325642</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>96</v>
+        <v>79</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="D14" s="11" t="n">
         <v>36149</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="n">
+      <c r="A15" s="10" t="n">
         <v>93224562</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D15" s="4" t="n">
         <v>32917</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1188,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1454,7 +1233,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>44275</v>
@@ -1485,7 +1264,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1536,7 +1315,7 @@
         <v>44640</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1561,7 +1340,7 @@
       <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1591,19 +1370,19 @@
     </row>
     <row r="2" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>44602.0</v>
@@ -1612,7 +1391,77 @@
         <v>44640.0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>44242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integral Test ok booking
</commit_message>
<xml_diff>
--- a/src/main/resources/dbAgencyTest.xlsx
+++ b/src/main/resources/dbAgencyTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoteles" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="98">
   <si>
     <t xml:space="preserve">Código Hotel</t>
   </si>
@@ -293,25 +293,34 @@
     <t xml:space="preserve">10/0L/2021</t>
   </si>
   <si>
+    <t>BH-0002</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Doble</t>
+  </si>
+  <si>
+    <t>$7200</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
     <t>CH-0003</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
     <t>Puerto Iguazú</t>
   </si>
   <si>
-    <t>Doble</t>
-  </si>
-  <si>
     <t>$6300</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -590,11 +599,11 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="2" customWidth="true" hidden="false" style="0" width="24.29" collapsed="true" outlineLevel="0"/>
     <col min="3" max="3" customWidth="true" hidden="false" style="0" width="18.86" collapsed="true" outlineLevel="0"/>
@@ -763,7 +772,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" customWidth="true" hidden="false" style="0" width="19.57" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="0" width="17.86" collapsed="true" outlineLevel="0"/>
@@ -920,7 +929,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="4" max="4" customWidth="true" hidden="false" style="0" width="25.71" collapsed="true" outlineLevel="0"/>
     <col min="5" max="5" customWidth="true" hidden="false" style="0" width="46.57" collapsed="true" outlineLevel="0"/>
@@ -1188,7 +1197,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1264,7 +1273,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1334,13 +1343,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1370,19 +1379,19 @@
     </row>
     <row r="2" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>44602.0</v>
@@ -1391,6 +1400,32 @@
         <v>44640.0</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>44239.0</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>44303.0</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1412,11 +1447,11 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>